<commit_message>
updated applications with SDKv5.00
</commit_message>
<xml_diff>
--- a/01_Head_count/Head_count_cam/exe/yolov3_cam/yolov3_cam_summary.xlsx
+++ b/01_Head_count/Head_count_cam/exe/yolov3_cam/yolov3_cam_summary.xlsx
@@ -834,7 +834,7 @@
         <v>416</v>
       </c>
       <c r="S6" t="n">
-        <v>3985</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="7" outlineLevel="1">
@@ -7246,7 +7246,7 @@
         </is>
       </c>
       <c r="S114" t="n">
-        <v>189106</v>
+        <v>186785</v>
       </c>
     </row>
     <row r="115">

</xml_diff>